<commit_message>
binary classification model rebuild with hyperparameter tuning
</commit_message>
<xml_diff>
--- a/reports/models_evaluations.xlsx
+++ b/reports/models_evaluations.xlsx
@@ -479,13 +479,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.98026388734893</v>
+        <v>0.9826994189117803</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9660183566433567</v>
+        <v>0.8130463286713286</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9730889879478289</v>
+        <v>0.8898588854341066</v>
       </c>
       <c r="E4" t="n">
         <v>9152</v>
@@ -500,13 +500,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.01892744479495268</v>
+        <v>0.0300453514739229</v>
       </c>
       <c r="C5" t="n">
-        <v>0.03260869565217391</v>
+        <v>0.2880434782608696</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02395209580838323</v>
+        <v>0.05441478439425051</v>
       </c>
       <c r="E5" t="n">
         <v>184</v>
@@ -521,16 +521,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9476221079691517</v>
+        <v>0.8026992287917738</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9476221079691517</v>
+        <v>0.8026992287917738</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9476221079691517</v>
+        <v>0.8026992287917738</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9476221079691517</v>
+        <v>0.8026992287917738</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
@@ -542,13 +542,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.4995956660719413</v>
+        <v>0.5063723851928515</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4993135261477653</v>
+        <v>0.5505449034660991</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4985205418781061</v>
+        <v>0.4721368349141786</v>
       </c>
       <c r="E7" t="n">
         <v>9336</v>
@@ -563,13 +563,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9613172393808569</v>
+        <v>0.9639238888765868</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9476221079691517</v>
+        <v>0.8026992287917738</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9543827767060061</v>
+        <v>0.8733934061505447</v>
       </c>
       <c r="E8" t="n">
         <v>9336</v>
@@ -588,10 +588,10 @@
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>0.532586129902706</v>
+        <v>0.5659587949414715</v>
       </c>
       <c r="G9" t="n">
-        <v>0.5</v>
+        <v>0.2943228781223297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small changes in forecast model
</commit_message>
<xml_diff>
--- a/reports/models_evaluations.xlsx
+++ b/reports/models_evaluations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,162 +436,49 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Model: classification_ann_model</t>
+          <t>Model: forecasting_prophet_splited_model</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>precision</t>
+          <t>mae</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>recall</t>
+          <t>mse</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>f1-score</t>
+          <t>rmse</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>support</t>
-        </is>
-      </c>
-      <c r="F3" s="1" t="inlineStr">
-        <is>
-          <t>roc_auc</t>
-        </is>
-      </c>
-      <c r="G3" s="1" t="inlineStr">
-        <is>
-          <t>threshold</t>
+          <t>mape</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>metrics</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9826994189117803</v>
+        <v>7612.847821239554</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8130463286713286</v>
+        <v>81425740.7853</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8898588854341066</v>
+        <v>9023.621267833663</v>
       </c>
       <c r="E4" t="n">
-        <v>9152</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.0300453514739229</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.2880434782608696</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.05441478439425051</v>
-      </c>
-      <c r="E5" t="n">
-        <v>184</v>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>accuracy</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.8026992287917738</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.8026992287917738</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.8026992287917738</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.8026992287917738</v>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>macro avg</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0.5063723851928515</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.5505449034660991</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.4721368349141786</v>
-      </c>
-      <c r="E7" t="n">
-        <v>9336</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>weighted avg</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.9639238888765868</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.8026992287917738</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.8733934061505447</v>
-      </c>
-      <c r="E8" t="n">
-        <v>9336</v>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>overall</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
-        <v>0.5659587949414715</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.2943228781223297</v>
+        <v>25.6161856113109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes in Prophet forecas model
</commit_message>
<xml_diff>
--- a/reports/models_evaluations.xlsx
+++ b/reports/models_evaluations.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="forecasting_prophet_splited_model" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,50 +434,43 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Model: forecasting_prophet_splited_model</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>mae</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>mse</t>
         </is>
       </c>
-      <c r="D3" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>rmse</t>
         </is>
       </c>
-      <c r="E3" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>mape</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>metrics</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B2" t="n">
         <v>7612.847821239554</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C2" t="n">
         <v>81425740.7853</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D2" t="n">
         <v>9023.621267833663</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E2" t="n">
         <v>25.6161856113109</v>
       </c>
     </row>

</xml_diff>